<commit_message>
Update previous worldometer excel files with new column names.
</commit_message>
<xml_diff>
--- a/worldometer/data/2020-03-27_worldometer_covid.xlsx
+++ b/worldometer/data/2020-03-27_worldometer_covid.xlsx
@@ -44,7 +44,7 @@
     <t xml:space="preserve">Active Cases</t>
   </si>
   <si>
-    <t xml:space="preserve">Serious Critical</t>
+    <t xml:space="preserve">Serious, Critical</t>
   </si>
   <si>
     <t xml:space="preserve">Total Cases / 1M Pop</t>
@@ -53,7 +53,7 @@
     <t xml:space="preserve">Deaths / 1M Pop</t>
   </si>
   <si>
-    <t xml:space="preserve">First Case</t>
+    <t xml:space="preserve">Reported First Case</t>
   </si>
   <si>
     <t xml:space="preserve">World</t>
@@ -942,13 +942,13 @@
       <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6411,13 +6411,13 @@
       <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>